<commit_message>
correct file about test case for OpenCart
</commit_message>
<xml_diff>
--- a/OpenCart.xlsx
+++ b/OpenCart.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="27">
   <si>
     <t>+</t>
   </si>
@@ -92,6 +92,9 @@
   </si>
   <si>
     <t>User login. Other fields are correct.</t>
+  </si>
+  <si>
+    <t>Avto</t>
   </si>
 </sst>
 </file>
@@ -250,7 +253,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -264,6 +267,43 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -277,40 +317,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -645,10 +651,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H25"/>
+  <dimension ref="B2:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -661,50 +667,50 @@
     <col min="14" max="14" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B2" s="5" t="s">
+    <row r="2" spans="2:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="6" t="s">
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="3" t="s">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="12" t="s">
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -720,255 +726,279 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="19" t="s">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="8"/>
+      <c r="C8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="20"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="C9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="20"/>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="9"/>
       <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="D10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1"/>
       <c r="F10" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="3" t="s">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="9"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="9"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="11" t="s">
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F12" s="21" t="s">
+      <c r="C14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F14" s="10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="6" t="s">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="7" t="s">
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="9"/>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="10"/>
-      <c r="C17" s="13" t="s">
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="22"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="5"/>
+      <c r="C19" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="15"/>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="12" t="s">
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="13"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="G20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="H20" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="11" t="s">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G19" s="21" t="s">
+      <c r="C21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G21" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="H19" s="21" t="s">
+      <c r="H21" s="10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="10"/>
-      <c r="C20" s="16" t="s">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="5"/>
+      <c r="C22" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="17"/>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="12" t="s">
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D23" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="F23" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G21" s="1" t="s">
+      <c r="G23" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H21" s="1" t="s">
+      <c r="H23" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="11" t="s">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G22" s="21" t="s">
+      <c r="C24" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G24" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="H22" s="21" t="s">
+      <c r="H24" s="10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="10"/>
-      <c r="C23" s="16" t="s">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="5"/>
+      <c r="C25" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="18"/>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="12" t="s">
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="16"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D24" s="1" t="s">
+      <c r="C26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="11" t="s">
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
+      <c r="C27" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="C17:H17"/>
-    <mergeCell ref="C20:H20"/>
-    <mergeCell ref="C23:H23"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B11:F11"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B15:H15"/>
-    <mergeCell ref="B16:H16"/>
+    <mergeCell ref="B17:H17"/>
+    <mergeCell ref="B18:H18"/>
+    <mergeCell ref="C19:H19"/>
+    <mergeCell ref="C22:H22"/>
+    <mergeCell ref="C25:H25"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="B13:F13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
create util and delete 1 test
</commit_message>
<xml_diff>
--- a/OpenCart.xlsx
+++ b/OpenCart.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="28">
   <si>
     <t>+</t>
   </si>
@@ -94,7 +94,10 @@
     <t>User login. Other fields are correct.</t>
   </si>
   <si>
-    <t>Avto</t>
+    <t>Name from 3 to 25</t>
+  </si>
+  <si>
+    <t>Review from 25 to 1000</t>
   </si>
 </sst>
 </file>
@@ -283,27 +286,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -317,6 +299,27 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -651,10 +654,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H27"/>
+  <dimension ref="B2:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -667,25 +670,25 @@
     <col min="14" max="14" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B2" s="18" t="s">
+    <row r="2" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="19" t="s">
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="6" t="s">
         <v>2</v>
@@ -700,16 +703,16 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="17" t="s">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="s">
         <v>7</v>
       </c>
@@ -726,279 +729,264 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="8"/>
-      <c r="C8" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="3" t="s">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="9"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F8" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="9"/>
       <c r="C10" s="1"/>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="1"/>
+      <c r="E10" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E10" s="1"/>
       <c r="F10" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="9"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1" t="s">
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F11" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="9"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="F13" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="15"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="5"/>
+      <c r="C18" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="18"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H20" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="5"/>
+      <c r="C21" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G23" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H23" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="5"/>
+      <c r="C24" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="21"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F14" s="10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="19"/>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="22"/>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="5"/>
-      <c r="C19" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="13"/>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="6" t="s">
+      <c r="D25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G21" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="H21" s="10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="5"/>
-      <c r="C22" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="15"/>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G24" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="H24" s="10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="5"/>
-      <c r="C25" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="15"/>
-      <c r="H25" s="16"/>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>24</v>
+      <c r="C26" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B27" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-    </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="C21:H21"/>
+    <mergeCell ref="C24:H24"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="B12:F12"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B16:H16"/>
     <mergeCell ref="B17:H17"/>
-    <mergeCell ref="B18:H18"/>
-    <mergeCell ref="C19:H19"/>
-    <mergeCell ref="C22:H22"/>
-    <mergeCell ref="C25:H25"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="C18:H18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>